<commit_message>
added script to fix 1 day high low wrong in test.py
</commit_message>
<xml_diff>
--- a/test/hl_test.xlsx
+++ b/test/hl_test.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -970,12 +970,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G136"/>
+  <dimension ref="A1:L136"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="735" activePane="bottomLeft"/>
       <selection activeCell="B16" sqref="B16:B52"/>
-      <selection pane="bottomLeft" activeCell="A11" sqref="A1:G136"/>
+      <selection pane="bottomLeft" activeCell="R15" sqref="R15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -985,7 +985,7 @@
     <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -1006,7 +1006,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
@@ -1028,8 +1028,20 @@
       <c r="G2" s="4">
         <v>583.20000000000005</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I2">
+        <v>646.9</v>
+      </c>
+      <c r="J2">
+        <v>628.5</v>
+      </c>
+      <c r="K2">
+        <v>646.9</v>
+      </c>
+      <c r="L2">
+        <v>628.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>7</v>
       </c>
@@ -1051,8 +1063,20 @@
       <c r="G3" s="5">
         <v>8142.05</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I3">
+        <v>5789.8</v>
+      </c>
+      <c r="J3">
+        <v>5585.5</v>
+      </c>
+      <c r="K3">
+        <v>5789.8</v>
+      </c>
+      <c r="L3">
+        <v>5585.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>8</v>
       </c>
@@ -1074,8 +1098,20 @@
       <c r="G4" s="5">
         <v>238.4</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I4">
+        <v>174.3</v>
+      </c>
+      <c r="J4">
+        <v>169.25</v>
+      </c>
+      <c r="K4">
+        <v>174.3</v>
+      </c>
+      <c r="L4">
+        <v>169.25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>9</v>
       </c>
@@ -1097,8 +1133,20 @@
       <c r="G5" s="5">
         <v>349.1</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I5">
+        <v>212.65</v>
+      </c>
+      <c r="J5">
+        <v>201</v>
+      </c>
+      <c r="K5">
+        <v>212.65</v>
+      </c>
+      <c r="L5">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
@@ -1120,8 +1168,20 @@
       <c r="G6" s="5">
         <v>3131.2</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I6">
+        <v>3143.4</v>
+      </c>
+      <c r="J6">
+        <v>3061.25</v>
+      </c>
+      <c r="K6">
+        <v>3143.4</v>
+      </c>
+      <c r="L6">
+        <v>3061.25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>11</v>
       </c>
@@ -1143,8 +1203,20 @@
       <c r="G7" s="5">
         <v>1453.85</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I7">
+        <v>1288.8499999999999</v>
+      </c>
+      <c r="J7">
+        <v>1256.6500000000001</v>
+      </c>
+      <c r="K7">
+        <v>1288.8499999999999</v>
+      </c>
+      <c r="L7">
+        <v>1256.6500000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>12</v>
       </c>
@@ -1166,8 +1238,20 @@
       <c r="G8" s="5">
         <v>6116.9</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I8">
+        <v>6233</v>
+      </c>
+      <c r="J8">
+        <v>6109.7</v>
+      </c>
+      <c r="K8">
+        <v>6233</v>
+      </c>
+      <c r="L8">
+        <v>6109.7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>13</v>
       </c>
@@ -1189,8 +1273,20 @@
       <c r="G9" s="5">
         <v>631.65</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I9">
+        <v>592.79999999999995</v>
+      </c>
+      <c r="J9">
+        <v>583.04999999999995</v>
+      </c>
+      <c r="K9">
+        <v>592.79999999999995</v>
+      </c>
+      <c r="L9">
+        <v>583.04999999999995</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>14</v>
       </c>
@@ -1212,8 +1308,20 @@
       <c r="G10" s="5">
         <v>7199.8</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I10">
+        <v>7018.95</v>
+      </c>
+      <c r="J10">
+        <v>6930.1</v>
+      </c>
+      <c r="K10">
+        <v>7018.95</v>
+      </c>
+      <c r="L10">
+        <v>6930.1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>15</v>
       </c>
@@ -1235,8 +1343,20 @@
       <c r="G11" s="5">
         <v>549.6</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I11">
+        <v>503.35</v>
+      </c>
+      <c r="J11">
+        <v>470.7</v>
+      </c>
+      <c r="K11">
+        <v>503.35</v>
+      </c>
+      <c r="L11">
+        <v>470.7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>16</v>
       </c>
@@ -1258,8 +1378,20 @@
       <c r="G12" s="5">
         <v>239.1</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I12">
+        <v>164.85</v>
+      </c>
+      <c r="J12">
+        <v>160.25</v>
+      </c>
+      <c r="K12">
+        <v>164.85</v>
+      </c>
+      <c r="L12">
+        <v>160.25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>17</v>
       </c>
@@ -1281,8 +1413,20 @@
       <c r="G13" s="5">
         <v>1987.25</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I13">
+        <v>2057.4</v>
+      </c>
+      <c r="J13">
+        <v>1956.8</v>
+      </c>
+      <c r="K13">
+        <v>2057.4</v>
+      </c>
+      <c r="L13">
+        <v>1956.8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>18</v>
       </c>
@@ -1304,8 +1448,20 @@
       <c r="G14" s="5">
         <v>7727.95</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I14">
+        <v>6060</v>
+      </c>
+      <c r="J14">
+        <v>5932.15</v>
+      </c>
+      <c r="K14">
+        <v>6060</v>
+      </c>
+      <c r="L14">
+        <v>5932.15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>19</v>
       </c>
@@ -1327,8 +1483,20 @@
       <c r="G15" s="5">
         <v>745.2</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I15">
+        <v>587.29999999999995</v>
+      </c>
+      <c r="J15">
+        <v>575.1</v>
+      </c>
+      <c r="K15">
+        <v>587.29999999999995</v>
+      </c>
+      <c r="L15">
+        <v>575.1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>20</v>
       </c>
@@ -1350,8 +1518,20 @@
       <c r="G16" s="5">
         <v>1457.35</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I16">
+        <v>1015.8</v>
+      </c>
+      <c r="J16">
+        <v>984.3</v>
+      </c>
+      <c r="K16">
+        <v>1015.8</v>
+      </c>
+      <c r="L16">
+        <v>984.3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>21</v>
       </c>
@@ -1373,8 +1553,20 @@
       <c r="G17" s="5">
         <v>1979.6</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I17">
+        <v>1589.6</v>
+      </c>
+      <c r="J17">
+        <v>1547.5</v>
+      </c>
+      <c r="K17">
+        <v>1589.6</v>
+      </c>
+      <c r="L17">
+        <v>1547.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>22</v>
       </c>
@@ -1396,8 +1588,20 @@
       <c r="G18" s="5">
         <v>7670.7</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I18">
+        <v>6578</v>
+      </c>
+      <c r="J18">
+        <v>6360</v>
+      </c>
+      <c r="K18">
+        <v>6578</v>
+      </c>
+      <c r="L18">
+        <v>6360</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>23</v>
       </c>
@@ -1419,8 +1623,20 @@
       <c r="G19" s="5">
         <v>3076.35</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I19">
+        <v>2286.15</v>
+      </c>
+      <c r="J19">
+        <v>2233</v>
+      </c>
+      <c r="K19">
+        <v>2286.15</v>
+      </c>
+      <c r="L19">
+        <v>2233</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>24</v>
       </c>
@@ -1442,8 +1658,20 @@
       <c r="G20" s="5">
         <v>649.5</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I20">
+        <v>361.95</v>
+      </c>
+      <c r="J20">
+        <v>350</v>
+      </c>
+      <c r="K20">
+        <v>361.95</v>
+      </c>
+      <c r="L20">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>25</v>
       </c>
@@ -1465,8 +1693,20 @@
       <c r="G21" s="5">
         <v>197.72</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I21">
+        <v>186</v>
+      </c>
+      <c r="J21">
+        <v>179.1</v>
+      </c>
+      <c r="K21">
+        <v>186</v>
+      </c>
+      <c r="L21">
+        <v>179.1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>26</v>
       </c>
@@ -1488,8 +1728,20 @@
       <c r="G22" s="5">
         <v>250.75</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I22">
+        <v>261.5</v>
+      </c>
+      <c r="J22">
+        <v>250.15</v>
+      </c>
+      <c r="K22">
+        <v>261.5</v>
+      </c>
+      <c r="L22">
+        <v>250.15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>27</v>
       </c>
@@ -1511,8 +1763,20 @@
       <c r="G23" s="5">
         <v>1445.6</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I23">
+        <v>1418.85</v>
+      </c>
+      <c r="J23">
+        <v>1386.45</v>
+      </c>
+      <c r="K23">
+        <v>1418.85</v>
+      </c>
+      <c r="L23">
+        <v>1386.45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>28</v>
       </c>
@@ -1534,8 +1798,20 @@
       <c r="G24" s="5">
         <v>286.45</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I24">
+        <v>196.75</v>
+      </c>
+      <c r="J24">
+        <v>179.1</v>
+      </c>
+      <c r="K24">
+        <v>196.75</v>
+      </c>
+      <c r="L24">
+        <v>179.1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>29</v>
       </c>
@@ -1557,8 +1833,20 @@
       <c r="G25" s="5">
         <v>1524.7</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I25">
+        <v>1130.6500000000001</v>
+      </c>
+      <c r="J25">
+        <v>1099.0999999999999</v>
+      </c>
+      <c r="K25">
+        <v>1130.6500000000001</v>
+      </c>
+      <c r="L25">
+        <v>1099.0999999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>30</v>
       </c>
@@ -1580,8 +1868,20 @@
       <c r="G26" s="5">
         <v>281.75</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I26">
+        <v>227.7</v>
+      </c>
+      <c r="J26">
+        <v>207.1</v>
+      </c>
+      <c r="K26">
+        <v>227.7</v>
+      </c>
+      <c r="L26">
+        <v>207.1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>31</v>
       </c>
@@ -1603,8 +1903,20 @@
       <c r="G27" s="5">
         <v>364.55</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I27">
+        <v>262.60000000000002</v>
+      </c>
+      <c r="J27">
+        <v>250.25</v>
+      </c>
+      <c r="K27">
+        <v>262.60000000000002</v>
+      </c>
+      <c r="L27">
+        <v>250.25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>32</v>
       </c>
@@ -1626,8 +1938,20 @@
       <c r="G28" s="5">
         <v>6331.9</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I28">
+        <v>5008.7</v>
+      </c>
+      <c r="J28">
+        <v>4912</v>
+      </c>
+      <c r="K28">
+        <v>5008.7</v>
+      </c>
+      <c r="L28">
+        <v>4912</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>33</v>
       </c>
@@ -1649,8 +1973,20 @@
       <c r="G29" s="5">
         <v>600.54999999999995</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I29">
+        <v>760.5</v>
+      </c>
+      <c r="J29">
+        <v>735.05</v>
+      </c>
+      <c r="K29">
+        <v>760.5</v>
+      </c>
+      <c r="L29">
+        <v>735.05</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>34</v>
       </c>
@@ -1672,8 +2008,20 @@
       <c r="G30" s="5">
         <v>112.05</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I30">
+        <v>554</v>
+      </c>
+      <c r="J30">
+        <v>529.75</v>
+      </c>
+      <c r="K30">
+        <v>554</v>
+      </c>
+      <c r="L30">
+        <v>529.75</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>35</v>
       </c>
@@ -1695,8 +2043,20 @@
       <c r="G31" s="5">
         <v>906.6</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I31">
+        <v>734.35</v>
+      </c>
+      <c r="J31">
+        <v>709.15</v>
+      </c>
+      <c r="K31">
+        <v>734.35</v>
+      </c>
+      <c r="L31">
+        <v>709.15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>36</v>
       </c>
@@ -1718,8 +2078,20 @@
       <c r="G32" s="5">
         <v>540.70000000000005</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I32">
+        <v>350.9</v>
+      </c>
+      <c r="J32">
+        <v>339.5</v>
+      </c>
+      <c r="K32">
+        <v>350.9</v>
+      </c>
+      <c r="L32">
+        <v>339.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>37</v>
       </c>
@@ -1741,8 +2113,14 @@
       <c r="G33" s="5">
         <v>1610.45</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K33">
+        <v>1086</v>
+      </c>
+      <c r="L33">
+        <v>1055.6500000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>38</v>
       </c>
@@ -1764,8 +2142,14 @@
       <c r="G34" s="5">
         <v>1655.15</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K34">
+        <v>1496.2</v>
+      </c>
+      <c r="L34">
+        <v>1466.05</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>39</v>
       </c>
@@ -1787,8 +2171,14 @@
       <c r="G35" s="5">
         <v>7046</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K35">
+        <v>6137.35</v>
+      </c>
+      <c r="L35">
+        <v>6008.3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>40</v>
       </c>
@@ -1810,8 +2200,14 @@
       <c r="G36" s="5">
         <v>922.3</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K36">
+        <v>872.4</v>
+      </c>
+      <c r="L36">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>41</v>
       </c>
@@ -1833,8 +2229,14 @@
       <c r="G37" s="5">
         <v>1689.9</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K37">
+        <v>1110</v>
+      </c>
+      <c r="L37">
+        <v>1059.75</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>42</v>
       </c>
@@ -1856,8 +2258,14 @@
       <c r="G38" s="5">
         <v>424.1</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K38">
+        <v>285.8</v>
+      </c>
+      <c r="L38">
+        <v>274.35000000000002</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
         <v>43</v>
       </c>
@@ -1879,8 +2287,14 @@
       <c r="G39" s="5">
         <v>3822.55</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K39">
+        <v>2737.1</v>
+      </c>
+      <c r="L39">
+        <v>2678.5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>44</v>
       </c>
@@ -1902,8 +2316,14 @@
       <c r="G40" s="5">
         <v>622.65</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K40">
+        <v>530.35</v>
+      </c>
+      <c r="L40">
+        <v>524.25</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
         <v>45</v>
       </c>
@@ -1925,8 +2345,14 @@
       <c r="G41" s="5">
         <v>1957</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K41">
+        <v>1893.9</v>
+      </c>
+      <c r="L41">
+        <v>1854.7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
         <v>46</v>
       </c>
@@ -1948,8 +2374,14 @@
       <c r="G42" s="5">
         <v>1083.05</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K42">
+        <v>495.5</v>
+      </c>
+      <c r="L42">
+        <v>466.1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>47</v>
       </c>
@@ -1971,8 +2403,14 @@
       <c r="G43" s="5">
         <v>2916.5</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K43">
+        <v>2123.5500000000002</v>
+      </c>
+      <c r="L43">
+        <v>2080</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
         <v>48</v>
       </c>
@@ -1994,8 +2432,14 @@
       <c r="G44" s="5">
         <v>130.91999999999999</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K44">
+        <v>127.7</v>
+      </c>
+      <c r="L44">
+        <v>122.75</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
         <v>49</v>
       </c>
@@ -2017,8 +2461,14 @@
       <c r="G45" s="5">
         <v>5428.65</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K45">
+        <v>3524.7</v>
+      </c>
+      <c r="L45">
+        <v>3455.05</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
         <v>50</v>
       </c>
@@ -2040,8 +2490,14 @@
       <c r="G46" s="5">
         <v>13919.15</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K46">
+        <v>6979.95</v>
+      </c>
+      <c r="L46">
+        <v>6722</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
         <v>51</v>
       </c>
@@ -2063,8 +2519,14 @@
       <c r="G47" s="5">
         <v>904.75</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K47">
+        <v>848.75</v>
+      </c>
+      <c r="L47">
+        <v>809.3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
         <v>52</v>
       </c>
@@ -2086,8 +2548,14 @@
       <c r="G48" s="5">
         <v>6733.65</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K48">
+        <v>6308.55</v>
+      </c>
+      <c r="L48">
+        <v>6214.5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
         <v>53</v>
       </c>
@@ -2109,8 +2577,14 @@
       <c r="G49" s="5">
         <v>4289.1000000000004</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K49">
+        <v>2773.95</v>
+      </c>
+      <c r="L49">
+        <v>2682.5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
         <v>54</v>
       </c>
@@ -2132,8 +2606,14 @@
       <c r="G50" s="5">
         <v>508.4</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K50">
+        <v>306.8</v>
+      </c>
+      <c r="L50">
+        <v>298.85000000000002</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
         <v>55</v>
       </c>
@@ -2155,8 +2635,14 @@
       <c r="G51" s="5">
         <v>1671.75</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K51">
+        <v>943.85</v>
+      </c>
+      <c r="L51">
+        <v>912.05</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
         <v>56</v>
       </c>
@@ -2178,8 +2664,14 @@
       <c r="G52" s="5">
         <v>1075</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K52">
+        <v>752</v>
+      </c>
+      <c r="L52">
+        <v>715.6</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
         <v>57</v>
       </c>
@@ -2201,8 +2693,14 @@
       <c r="G53" s="5">
         <v>680.85</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K53">
+        <v>630.9</v>
+      </c>
+      <c r="L53">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
         <v>58</v>
       </c>
@@ -2224,8 +2722,14 @@
       <c r="G54" s="5">
         <v>1383.35</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K54">
+        <v>1223.8</v>
+      </c>
+      <c r="L54">
+        <v>1203.7</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
         <v>59</v>
       </c>
@@ -2247,8 +2751,14 @@
       <c r="G55" s="5">
         <v>3209.15</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K55">
+        <v>2234.1999999999998</v>
+      </c>
+      <c r="L55">
+        <v>2157.9499999999998</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
         <v>60</v>
       </c>
@@ -2270,8 +2780,14 @@
       <c r="G56" s="5">
         <v>558.5</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K56">
+        <v>424.85</v>
+      </c>
+      <c r="L56">
+        <v>410.4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
         <v>61</v>
       </c>
@@ -2293,8 +2809,14 @@
       <c r="G57" s="5">
         <v>2800.05</v>
       </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K57">
+        <v>2208.9</v>
+      </c>
+      <c r="L57">
+        <v>2165.0500000000002</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
         <v>62</v>
       </c>
@@ -2316,8 +2838,14 @@
       <c r="G58" s="5">
         <v>621.20000000000005</v>
       </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K58">
+        <v>546.95000000000005</v>
+      </c>
+      <c r="L58">
+        <v>528.54999999999995</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
         <v>63</v>
       </c>
@@ -2339,8 +2867,14 @@
       <c r="G59" s="5">
         <v>4440.95</v>
       </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K59">
+        <v>3182.55</v>
+      </c>
+      <c r="L59">
+        <v>3006</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
         <v>64</v>
       </c>
@@ -2362,8 +2896,14 @@
       <c r="G60" s="5">
         <v>2020</v>
       </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K60">
+        <v>1520.3</v>
+      </c>
+      <c r="L60">
+        <v>1476.05</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
         <v>65</v>
       </c>
@@ -2385,8 +2925,14 @@
       <c r="G61" s="5">
         <v>1802.75</v>
       </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K61">
+        <v>1677</v>
+      </c>
+      <c r="L61">
+        <v>1642.85</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
         <v>66</v>
       </c>
@@ -2408,8 +2954,14 @@
       <c r="G62" s="5">
         <v>4347.6000000000004</v>
       </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K62">
+        <v>3831.45</v>
+      </c>
+      <c r="L62">
+        <v>3680</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
         <v>67</v>
       </c>
@@ -2431,8 +2983,14 @@
       <c r="G63" s="5">
         <v>719.8</v>
       </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K63">
+        <v>634.79999999999995</v>
+      </c>
+      <c r="L63">
+        <v>611.29999999999995</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
         <v>68</v>
       </c>
@@ -2454,8 +3012,14 @@
       <c r="G64" s="5">
         <v>752.05</v>
       </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K64">
+        <v>534.04999999999995</v>
+      </c>
+      <c r="L64">
+        <v>517.5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
         <v>69</v>
       </c>
@@ -2477,8 +3041,14 @@
       <c r="G65" s="5">
         <v>341.7</v>
       </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K65">
+        <v>275.60000000000002</v>
+      </c>
+      <c r="L65">
+        <v>255.75</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
         <v>70</v>
       </c>
@@ -2500,8 +3070,14 @@
       <c r="G66" s="5">
         <v>2175.4</v>
       </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K66">
+        <v>1688.75</v>
+      </c>
+      <c r="L66">
+        <v>1633.05</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
         <v>71</v>
       </c>
@@ -2523,8 +3099,14 @@
       <c r="G67" s="5">
         <v>781.65</v>
       </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K67">
+        <v>579</v>
+      </c>
+      <c r="L67">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
         <v>72</v>
       </c>
@@ -2546,8 +3128,14 @@
       <c r="G68" s="5">
         <v>205.82</v>
       </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K68">
+        <v>138.25</v>
+      </c>
+      <c r="L68">
+        <v>133.4</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
         <v>73</v>
       </c>
@@ -2569,8 +3157,14 @@
       <c r="G69" s="5">
         <v>569.04999999999995</v>
       </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K69">
+        <v>414</v>
+      </c>
+      <c r="L69">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
         <v>74</v>
       </c>
@@ -2592,8 +3186,14 @@
       <c r="G70" s="5">
         <v>686.55</v>
       </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K70">
+        <v>565.9</v>
+      </c>
+      <c r="L70">
+        <v>549.95000000000005</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
         <v>75</v>
       </c>
@@ -2615,8 +3215,14 @@
       <c r="G71" s="5">
         <v>364.9</v>
       </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K71">
+        <v>207</v>
+      </c>
+      <c r="L71">
+        <v>199.2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
         <v>76</v>
       </c>
@@ -2638,8 +3244,14 @@
       <c r="G72" s="5">
         <v>2991.25</v>
       </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K72">
+        <v>2661.8</v>
+      </c>
+      <c r="L72">
+        <v>2599.25</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
         <v>77</v>
       </c>
@@ -2661,8 +3273,14 @@
       <c r="G73" s="5">
         <v>4825</v>
       </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K73">
+        <v>3215.9</v>
+      </c>
+      <c r="L73">
+        <v>3135</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
         <v>78</v>
       </c>
@@ -2684,8 +3302,14 @@
       <c r="G74" s="5">
         <v>1444.95</v>
       </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K74">
+        <v>1489.5</v>
+      </c>
+      <c r="L74">
+        <v>1456.7</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
         <v>79</v>
       </c>
@@ -2707,8 +3331,14 @@
       <c r="G75" s="5">
         <v>393.85</v>
       </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K75">
+        <v>252.4</v>
+      </c>
+      <c r="L75">
+        <v>241.2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
         <v>80</v>
       </c>
@@ -2730,8 +3360,14 @@
       <c r="G76" s="5">
         <v>947.7</v>
       </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K76">
+        <v>1199</v>
+      </c>
+      <c r="L76">
+        <v>1101</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
         <v>81</v>
       </c>
@@ -2753,8 +3389,14 @@
       <c r="G77" s="5">
         <v>1499.75</v>
       </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K77">
+        <v>1194.9000000000001</v>
+      </c>
+      <c r="L77">
+        <v>1143.9000000000001</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
         <v>82</v>
       </c>
@@ -2776,8 +3418,14 @@
       <c r="G78" s="5">
         <v>1038.6500000000001</v>
       </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K78">
+        <v>783.1</v>
+      </c>
+      <c r="L78">
+        <v>760.9</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
         <v>83</v>
       </c>
@@ -2799,8 +3447,14 @@
       <c r="G79" s="5">
         <v>4635</v>
       </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K79">
+        <v>4122.1499999999996</v>
+      </c>
+      <c r="L79">
+        <v>4010.05</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
         <v>84</v>
       </c>
@@ -2822,8 +3476,14 @@
       <c r="G80" s="5">
         <v>1022.8</v>
       </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K80">
+        <v>790.2</v>
+      </c>
+      <c r="L80">
+        <v>774.55</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
         <v>85</v>
       </c>
@@ -2845,8 +3505,14 @@
       <c r="G81" s="5">
         <v>675</v>
       </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K81">
+        <v>453.25</v>
+      </c>
+      <c r="L81">
+        <v>439.9</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
         <v>86</v>
       </c>
@@ -2868,8 +3534,14 @@
       <c r="G82" s="5">
         <v>1864.15</v>
       </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K82">
+        <v>1756</v>
+      </c>
+      <c r="L82">
+        <v>1721.2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
         <v>87</v>
       </c>
@@ -2891,8 +3563,14 @@
       <c r="G83" s="5">
         <v>3323.1</v>
       </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K83">
+        <v>2065</v>
+      </c>
+      <c r="L83">
+        <v>2013.2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
         <v>88</v>
       </c>
@@ -2914,8 +3592,14 @@
       <c r="G84" s="5">
         <v>461.5</v>
       </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K84">
+        <v>403.1</v>
+      </c>
+      <c r="L84">
+        <v>389.5</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
         <v>89</v>
       </c>
@@ -2937,8 +3621,14 @@
       <c r="G85" s="5">
         <v>666</v>
       </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K85">
+        <v>594.75</v>
+      </c>
+      <c r="L85">
+        <v>575.25</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
         <v>90</v>
       </c>
@@ -2960,8 +3650,14 @@
       <c r="G86" s="5">
         <v>6243.95</v>
       </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K86">
+        <v>5249.95</v>
+      </c>
+      <c r="L86">
+        <v>5170</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
         <v>91</v>
       </c>
@@ -2983,8 +3679,14 @@
       <c r="G87" s="5">
         <v>5357.4</v>
       </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K87">
+        <v>5437.85</v>
+      </c>
+      <c r="L87">
+        <v>5242.2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
         <v>92</v>
       </c>
@@ -3006,8 +3708,14 @@
       <c r="G88" s="5">
         <v>2203.6999999999998</v>
       </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K88">
+        <v>1674</v>
+      </c>
+      <c r="L88">
+        <v>1614</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
         <v>93</v>
       </c>
@@ -3029,8 +3737,14 @@
       <c r="G89" s="5">
         <v>337.75</v>
       </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K89">
+        <v>269.7</v>
+      </c>
+      <c r="L89">
+        <v>260.10000000000002</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
         <v>94</v>
       </c>
@@ -3052,8 +3766,14 @@
       <c r="G90" s="5">
         <v>196.51</v>
       </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K90">
+        <v>167.35</v>
+      </c>
+      <c r="L90">
+        <v>161.65</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
         <v>95</v>
       </c>
@@ -3075,8 +3795,14 @@
       <c r="G91" s="5">
         <v>692</v>
       </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K91">
+        <v>509.65</v>
+      </c>
+      <c r="L91">
+        <v>496.5</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
         <v>96</v>
       </c>
@@ -3098,8 +3824,14 @@
       <c r="G92" s="5">
         <v>1600.05</v>
       </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K92">
+        <v>1162</v>
+      </c>
+      <c r="L92">
+        <v>1108.45</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
         <v>97</v>
       </c>
@@ -3121,8 +3853,14 @@
       <c r="G93" s="5">
         <v>5787.3</v>
       </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K93">
+        <v>3277.45</v>
+      </c>
+      <c r="L93">
+        <v>3075.25</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
         <v>98</v>
       </c>
@@ -3144,8 +3882,14 @@
       <c r="G94" s="5">
         <v>2191.8000000000002</v>
       </c>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K94">
+        <v>1627.95</v>
+      </c>
+      <c r="L94">
+        <v>1580.1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
         <v>99</v>
       </c>
@@ -3167,8 +3911,14 @@
       <c r="G95" s="5">
         <v>1187.1500000000001</v>
       </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K95">
+        <v>994</v>
+      </c>
+      <c r="L95">
+        <v>952.9</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
         <v>100</v>
       </c>
@@ -3190,8 +3940,14 @@
       <c r="G96" s="5">
         <v>1947.55</v>
       </c>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K96">
+        <v>1279.6500000000001</v>
+      </c>
+      <c r="L96">
+        <v>1243</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
         <v>101</v>
       </c>
@@ -3213,8 +3969,14 @@
       <c r="G97" s="5">
         <v>3038.25</v>
       </c>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K97">
+        <v>2502</v>
+      </c>
+      <c r="L97">
+        <v>2455.85</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
         <v>102</v>
       </c>
@@ -3236,8 +3998,14 @@
       <c r="G98" s="5">
         <v>2003.3</v>
       </c>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K98">
+        <v>1368.9</v>
+      </c>
+      <c r="L98">
+        <v>1328.85</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
         <v>103</v>
       </c>
@@ -3259,8 +4027,14 @@
       <c r="G99" s="5">
         <v>662.85</v>
       </c>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K99">
+        <v>488.7</v>
+      </c>
+      <c r="L99">
+        <v>450.5</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
         <v>104</v>
       </c>
@@ -3282,8 +4056,14 @@
       <c r="G100" s="5">
         <v>8197.85</v>
       </c>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K100">
+        <v>5280</v>
+      </c>
+      <c r="L100">
+        <v>5161.3</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
         <v>105</v>
       </c>
@@ -3305,8 +4085,14 @@
       <c r="G101" s="5">
         <v>3466.6</v>
       </c>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K101">
+        <v>3010.05</v>
+      </c>
+      <c r="L101">
+        <v>2964.3</v>
+      </c>
+    </row>
+    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
         <v>106</v>
       </c>
@@ -3328,8 +4114,14 @@
       <c r="G102" s="5">
         <v>243.38</v>
       </c>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K102">
+        <v>204.5</v>
+      </c>
+      <c r="L102">
+        <v>190.35</v>
+      </c>
+    </row>
+    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
         <v>107</v>
       </c>
@@ -3351,8 +4143,14 @@
       <c r="G103" s="5">
         <v>444.6</v>
       </c>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K103">
+        <v>326.05</v>
+      </c>
+      <c r="L103">
+        <v>305.75</v>
+      </c>
+    </row>
+    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
         <v>108</v>
       </c>
@@ -3374,8 +4172,14 @@
       <c r="G104" s="5">
         <v>1898.75</v>
       </c>
-    </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K104">
+        <v>1343.95</v>
+      </c>
+      <c r="L104">
+        <v>1297.25</v>
+      </c>
+    </row>
+    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
         <v>109</v>
       </c>
@@ -3397,8 +4201,14 @@
       <c r="G105" s="5">
         <v>299</v>
       </c>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K105">
+        <v>266.39999999999998</v>
+      </c>
+      <c r="L105">
+        <v>248.9</v>
+      </c>
+    </row>
+    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A106" s="5" t="s">
         <v>110</v>
       </c>
@@ -3420,8 +4230,14 @@
       <c r="G106" s="5">
         <v>1112</v>
       </c>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K106">
+        <v>843.5</v>
+      </c>
+      <c r="L106">
+        <v>814.8</v>
+      </c>
+    </row>
+    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
         <v>111</v>
       </c>
@@ -3443,8 +4259,14 @@
       <c r="G107" s="5">
         <v>5472.6</v>
       </c>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K107">
+        <v>8454.85</v>
+      </c>
+      <c r="L107">
+        <v>8180</v>
+      </c>
+    </row>
+    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A108" s="5" t="s">
         <v>112</v>
       </c>
@@ -3466,8 +4288,14 @@
       <c r="G108" s="5">
         <v>342.15</v>
       </c>
-    </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K108">
+        <v>269.60000000000002</v>
+      </c>
+      <c r="L108">
+        <v>258.05</v>
+      </c>
+    </row>
+    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A109" s="5" t="s">
         <v>113</v>
       </c>
@@ -3489,8 +4317,14 @@
       <c r="G109" s="5">
         <v>3365.85</v>
       </c>
-    </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K109">
+        <v>2894</v>
+      </c>
+      <c r="L109">
+        <v>2819</v>
+      </c>
+    </row>
+    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
         <v>114</v>
       </c>
@@ -3512,8 +4346,14 @@
       <c r="G110" s="5">
         <v>6928.65</v>
       </c>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K110">
+        <v>4918.05</v>
+      </c>
+      <c r="L110">
+        <v>4775</v>
+      </c>
+    </row>
+    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A111" s="5" t="s">
         <v>115</v>
       </c>
@@ -3535,8 +4375,14 @@
       <c r="G111" s="5">
         <v>354.3</v>
       </c>
-    </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K111">
+        <v>272</v>
+      </c>
+      <c r="L111">
+        <v>257.64999999999998</v>
+      </c>
+    </row>
+    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A112" s="5" t="s">
         <v>116</v>
       </c>
@@ -3558,8 +4404,14 @@
       <c r="G112" s="5">
         <v>179.8</v>
       </c>
-    </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K112">
+        <v>162.30000000000001</v>
+      </c>
+      <c r="L112">
+        <v>156.35</v>
+      </c>
+    </row>
+    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A113" s="5" t="s">
         <v>117</v>
       </c>
@@ -3581,8 +4433,14 @@
       <c r="G113" s="5">
         <v>871.85</v>
       </c>
-    </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K113">
+        <v>809</v>
+      </c>
+      <c r="L113">
+        <v>792.7</v>
+      </c>
+    </row>
+    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A114" s="5" t="s">
         <v>118</v>
       </c>
@@ -3604,8 +4462,14 @@
       <c r="G114" s="5">
         <v>204.8</v>
       </c>
-    </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K114">
+        <v>230.65</v>
+      </c>
+      <c r="L114">
+        <v>222.25</v>
+      </c>
+    </row>
+    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A115" s="5" t="s">
         <v>119</v>
       </c>
@@ -3627,8 +4491,14 @@
       <c r="G115" s="5">
         <v>563.54999999999995</v>
       </c>
-    </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K115">
+        <v>466.5</v>
+      </c>
+      <c r="L115">
+        <v>430.35</v>
+      </c>
+    </row>
+    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A116" s="5" t="s">
         <v>120</v>
       </c>
@@ -3650,8 +4520,14 @@
       <c r="G116" s="5">
         <v>775.7</v>
       </c>
-    </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K116">
+        <v>704.65</v>
+      </c>
+      <c r="L116">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A117" s="5" t="s">
         <v>121</v>
       </c>
@@ -3673,8 +4549,14 @@
       <c r="G117" s="5">
         <v>1844.55</v>
       </c>
-    </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K117">
+        <v>1504.95</v>
+      </c>
+      <c r="L117">
+        <v>1481.1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A118" s="5" t="s">
         <v>122</v>
       </c>
@@ -3696,8 +4578,14 @@
       <c r="G118" s="5">
         <v>7337.2</v>
       </c>
-    </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K118">
+        <v>4820.6000000000004</v>
+      </c>
+      <c r="L118">
+        <v>4682.1000000000004</v>
+      </c>
+    </row>
+    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A119" s="5" t="s">
         <v>123</v>
       </c>
@@ -3719,8 +4607,14 @@
       <c r="G119" s="5">
         <v>2464.85</v>
       </c>
-    </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K119">
+        <v>2449.9</v>
+      </c>
+      <c r="L119">
+        <v>2404.4</v>
+      </c>
+    </row>
+    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A120" s="5" t="s">
         <v>124</v>
       </c>
@@ -3742,8 +4636,14 @@
       <c r="G120" s="5">
         <v>1377.6</v>
       </c>
-    </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K120">
+        <v>799.2</v>
+      </c>
+      <c r="L120">
+        <v>766.85</v>
+      </c>
+    </row>
+    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A121" s="5" t="s">
         <v>125</v>
       </c>
@@ -3765,8 +4665,14 @@
       <c r="G121" s="5">
         <v>1920.3</v>
       </c>
-    </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K121">
+        <v>1573.5</v>
+      </c>
+      <c r="L121">
+        <v>1541.2</v>
+      </c>
+    </row>
+    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A122" s="5" t="s">
         <v>126</v>
       </c>
@@ -3788,8 +4694,14 @@
       <c r="G122" s="5">
         <v>903.5</v>
       </c>
-    </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K122">
+        <v>687.9</v>
+      </c>
+      <c r="L122">
+        <v>671.9</v>
+      </c>
+    </row>
+    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A123" s="5" t="s">
         <v>127</v>
       </c>
@@ -3811,8 +4723,14 @@
       <c r="G123" s="5">
         <v>2153.85</v>
       </c>
-    </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K123">
+        <v>1954.6</v>
+      </c>
+      <c r="L123">
+        <v>1896.55</v>
+      </c>
+    </row>
+    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A124" s="5" t="s">
         <v>128</v>
       </c>
@@ -3834,8 +4752,14 @@
       <c r="G124" s="5">
         <v>980</v>
       </c>
-    </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K124">
+        <v>979.75</v>
+      </c>
+      <c r="L124">
+        <v>940</v>
+      </c>
+    </row>
+    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A125" s="5" t="s">
         <v>129</v>
       </c>
@@ -3857,8 +4781,14 @@
       <c r="G125" s="5">
         <v>1628.2</v>
       </c>
-    </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K125">
+        <v>1293</v>
+      </c>
+      <c r="L125">
+        <v>1268.5</v>
+      </c>
+    </row>
+    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A126" s="5" t="s">
         <v>130</v>
       </c>
@@ -3880,8 +4810,14 @@
       <c r="G126" s="5">
         <v>3382.95</v>
       </c>
-    </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K126">
+        <v>2711.1</v>
+      </c>
+      <c r="L126">
+        <v>2577</v>
+      </c>
+    </row>
+    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A127" s="5" t="s">
         <v>131</v>
       </c>
@@ -3903,8 +4839,14 @@
       <c r="G127" s="5">
         <v>1863</v>
       </c>
-    </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K127">
+        <v>1185</v>
+      </c>
+      <c r="L127">
+        <v>1115.45</v>
+      </c>
+    </row>
+    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A128" s="5" t="s">
         <v>132</v>
       </c>
@@ -3926,8 +4868,14 @@
       <c r="G128" s="5">
         <v>7559.85</v>
       </c>
-    </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K128">
+        <v>4145</v>
+      </c>
+      <c r="L128">
+        <v>3981.25</v>
+      </c>
+    </row>
+    <row r="129" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A129" s="5" t="s">
         <v>133</v>
       </c>
@@ -3949,8 +4897,14 @@
       <c r="G129" s="5">
         <v>2853.55</v>
       </c>
-    </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K129">
+        <v>2159</v>
+      </c>
+      <c r="L129">
+        <v>2054.9499999999998</v>
+      </c>
+    </row>
+    <row r="130" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A130" s="5" t="s">
         <v>134</v>
       </c>
@@ -3972,8 +4926,14 @@
       <c r="G130" s="5">
         <v>2173.1</v>
       </c>
-    </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K130">
+        <v>1745.95</v>
+      </c>
+      <c r="L130">
+        <v>1696.25</v>
+      </c>
+    </row>
+    <row r="131" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A131" s="5" t="s">
         <v>135</v>
       </c>
@@ -3995,8 +4955,14 @@
       <c r="G131" s="5">
         <v>11798.8</v>
       </c>
-    </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K131">
+        <v>9750.9</v>
+      </c>
+      <c r="L131">
+        <v>9543.7999999999993</v>
+      </c>
+    </row>
+    <row r="132" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A132" s="5" t="s">
         <v>136</v>
       </c>
@@ -4018,8 +4984,14 @@
       <c r="G132" s="5">
         <v>617.4</v>
       </c>
-    </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K132">
+        <v>477.5</v>
+      </c>
+      <c r="L132">
+        <v>459.45</v>
+      </c>
+    </row>
+    <row r="133" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A133" s="5" t="s">
         <v>137</v>
       </c>
@@ -4041,8 +5013,14 @@
       <c r="G133" s="5">
         <v>511.05</v>
       </c>
-    </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K133">
+        <v>266</v>
+      </c>
+      <c r="L133">
+        <v>255.15</v>
+      </c>
+    </row>
+    <row r="134" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A134" s="5" t="s">
         <v>138</v>
       </c>
@@ -4064,8 +5042,14 @@
       <c r="G134" s="5">
         <v>1850.65</v>
       </c>
-    </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K134">
+        <v>1073.6500000000001</v>
+      </c>
+      <c r="L134">
+        <v>1050.05</v>
+      </c>
+    </row>
+    <row r="135" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A135" s="5" t="s">
         <v>139</v>
       </c>
@@ -4087,8 +5071,14 @@
       <c r="G135" s="5">
         <v>138.6</v>
       </c>
-    </row>
-    <row r="136" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K135">
+        <v>149.1</v>
+      </c>
+      <c r="L135">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="136" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A136" s="6" t="s">
         <v>140</v>
       </c>
@@ -4109,6 +5099,12 @@
       </c>
       <c r="G136" s="6">
         <v>1072.5999999999999</v>
+      </c>
+      <c r="K136">
+        <v>994.65</v>
+      </c>
+      <c r="L136">
+        <v>971.25</v>
       </c>
     </row>
   </sheetData>
@@ -4119,10 +5115,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G136"/>
+  <dimension ref="A1:G143"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4156,10 +5152,10 @@
         <v>6</v>
       </c>
       <c r="B2" s="7">
-        <v>643.79999999999995</v>
+        <v>646.9</v>
       </c>
       <c r="C2" s="9">
-        <v>626</v>
+        <v>628.5</v>
       </c>
       <c r="D2" s="12"/>
       <c r="E2" s="4"/>
@@ -4171,10 +5167,10 @@
         <v>7</v>
       </c>
       <c r="B3" s="19">
-        <v>8144.7</v>
+        <v>5789.8</v>
       </c>
       <c r="C3" s="20">
-        <v>7801.05</v>
+        <v>5585.5</v>
       </c>
       <c r="D3" s="13"/>
       <c r="E3" s="5"/>
@@ -4186,10 +5182,10 @@
         <v>8</v>
       </c>
       <c r="B4" s="8">
-        <v>232.55</v>
+        <v>174.3</v>
       </c>
       <c r="C4" s="10">
-        <v>217</v>
+        <v>169.25</v>
       </c>
       <c r="D4" s="13"/>
       <c r="E4" s="5"/>
@@ -4201,10 +5197,10 @@
         <v>9</v>
       </c>
       <c r="B5" s="8">
-        <v>325.5</v>
+        <v>212.65</v>
       </c>
       <c r="C5" s="10">
-        <v>307</v>
+        <v>201</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="5"/>
@@ -4216,10 +5212,10 @@
         <v>10</v>
       </c>
       <c r="B6" s="19">
-        <v>3222.4</v>
+        <v>3143.4</v>
       </c>
       <c r="C6" s="20">
-        <v>3137.15</v>
+        <v>3061.25</v>
       </c>
       <c r="D6" s="13"/>
       <c r="E6" s="5"/>
@@ -4231,10 +5227,10 @@
         <v>11</v>
       </c>
       <c r="B7" s="19">
-        <v>1472.85</v>
+        <v>1288.8499999999999</v>
       </c>
       <c r="C7" s="20">
-        <v>1448</v>
+        <v>1256.6500000000001</v>
       </c>
       <c r="D7" s="13"/>
       <c r="E7" s="5"/>
@@ -4246,10 +5242,10 @@
         <v>12</v>
       </c>
       <c r="B8" s="19">
-        <v>4889.1000000000004</v>
+        <v>6233</v>
       </c>
       <c r="C8" s="20">
-        <v>4775</v>
+        <v>6109.7</v>
       </c>
       <c r="D8" s="13"/>
       <c r="E8" s="5"/>
@@ -4261,10 +5257,10 @@
         <v>13</v>
       </c>
       <c r="B9" s="8">
-        <v>622.25</v>
+        <v>592.79999999999995</v>
       </c>
       <c r="C9" s="10">
-        <v>603.75</v>
+        <v>583.04999999999995</v>
       </c>
       <c r="D9" s="13"/>
       <c r="E9" s="5"/>
@@ -4276,10 +5272,10 @@
         <v>14</v>
       </c>
       <c r="B10" s="19">
-        <v>5975</v>
+        <v>7018.95</v>
       </c>
       <c r="C10" s="20">
-        <v>5900</v>
+        <v>6930.1</v>
       </c>
       <c r="D10" s="13"/>
       <c r="E10" s="5"/>
@@ -4291,10 +5287,10 @@
         <v>15</v>
       </c>
       <c r="B11" s="8">
-        <v>474</v>
+        <v>503.35</v>
       </c>
       <c r="C11" s="10">
-        <v>466.25</v>
+        <v>470.7</v>
       </c>
       <c r="D11" s="13"/>
       <c r="E11" s="5"/>
@@ -4306,10 +5302,10 @@
         <v>16</v>
       </c>
       <c r="B12" s="8">
-        <v>231.05</v>
+        <v>164.85</v>
       </c>
       <c r="C12" s="10">
-        <v>223.55</v>
+        <v>160.25</v>
       </c>
       <c r="D12" s="13"/>
       <c r="E12" s="5"/>
@@ -4321,10 +5317,10 @@
         <v>17</v>
       </c>
       <c r="B13" s="19">
-        <v>2184</v>
+        <v>2057.4</v>
       </c>
       <c r="C13" s="20">
-        <v>2110.5</v>
+        <v>1956.8</v>
       </c>
       <c r="D13" s="13"/>
       <c r="E13" s="5"/>
@@ -4336,10 +5332,10 @@
         <v>18</v>
       </c>
       <c r="B14" s="19">
-        <v>5855.9</v>
+        <v>6060</v>
       </c>
       <c r="C14" s="20">
-        <v>5765</v>
+        <v>5932.15</v>
       </c>
       <c r="D14" s="13"/>
       <c r="E14" s="5"/>
@@ -4351,10 +5347,10 @@
         <v>19</v>
       </c>
       <c r="B15" s="8">
-        <v>678.5</v>
+        <v>587.29999999999995</v>
       </c>
       <c r="C15" s="10">
-        <v>654</v>
+        <v>575.1</v>
       </c>
       <c r="D15" s="13"/>
       <c r="E15" s="5"/>
@@ -4366,10 +5362,10 @@
         <v>20</v>
       </c>
       <c r="B16" s="19">
-        <v>1270.95</v>
+        <v>1015.8</v>
       </c>
       <c r="C16" s="20">
-        <v>1233.8499999999999</v>
+        <v>984.3</v>
       </c>
       <c r="D16" s="13"/>
       <c r="E16" s="5"/>
@@ -4381,10 +5377,10 @@
         <v>21</v>
       </c>
       <c r="B17" s="19">
-        <v>1541.5</v>
+        <v>1589.6</v>
       </c>
       <c r="C17" s="20">
-        <v>1510.8</v>
+        <v>1547.5</v>
       </c>
       <c r="D17" s="13"/>
       <c r="E17" s="5"/>
@@ -4396,10 +5392,10 @@
         <v>22</v>
       </c>
       <c r="B18" s="19">
-        <v>7012.95</v>
+        <v>6578</v>
       </c>
       <c r="C18" s="20">
-        <v>6822.3</v>
+        <v>6360</v>
       </c>
       <c r="D18" s="13"/>
       <c r="E18" s="5"/>
@@ -4411,10 +5407,10 @@
         <v>23</v>
       </c>
       <c r="B19" s="19">
-        <v>3155</v>
+        <v>2286.15</v>
       </c>
       <c r="C19" s="20">
-        <v>3075.5</v>
+        <v>2233</v>
       </c>
       <c r="D19" s="13"/>
       <c r="E19" s="5"/>
@@ -4426,10 +5422,10 @@
         <v>24</v>
       </c>
       <c r="B20" s="8">
-        <v>394</v>
+        <v>361.95</v>
       </c>
       <c r="C20" s="10">
-        <v>385.25</v>
+        <v>350</v>
       </c>
       <c r="D20" s="13"/>
       <c r="E20" s="5"/>
@@ -4441,10 +5437,10 @@
         <v>25</v>
       </c>
       <c r="B21" s="8">
-        <v>194.8</v>
+        <v>186</v>
       </c>
       <c r="C21" s="10">
-        <v>190.35</v>
+        <v>179.1</v>
       </c>
       <c r="D21" s="13"/>
       <c r="E21" s="5"/>
@@ -4456,10 +5452,10 @@
         <v>26</v>
       </c>
       <c r="B22" s="8">
-        <v>274</v>
+        <v>261.5</v>
       </c>
       <c r="C22" s="10">
-        <v>261.45</v>
+        <v>250.15</v>
       </c>
       <c r="D22" s="13"/>
       <c r="E22" s="5"/>
@@ -4471,10 +5467,10 @@
         <v>27</v>
       </c>
       <c r="B23" s="8">
-        <v>1465</v>
+        <v>1418.85</v>
       </c>
       <c r="C23" s="10">
-        <v>1415.95</v>
+        <v>1386.45</v>
       </c>
       <c r="D23" s="13"/>
       <c r="E23" s="5"/>
@@ -4486,10 +5482,10 @@
         <v>28</v>
       </c>
       <c r="B24" s="8">
-        <v>281.5</v>
+        <v>196.75</v>
       </c>
       <c r="C24" s="10">
-        <v>267</v>
+        <v>179.1</v>
       </c>
       <c r="D24" s="13"/>
       <c r="E24" s="5"/>
@@ -4501,10 +5497,10 @@
         <v>29</v>
       </c>
       <c r="B25" s="8">
-        <v>1578.85</v>
+        <v>1130.6500000000001</v>
       </c>
       <c r="C25" s="10">
-        <v>1497.1</v>
+        <v>1099.0999999999999</v>
       </c>
       <c r="D25" s="13"/>
       <c r="E25" s="5"/>
@@ -4516,10 +5512,10 @@
         <v>30</v>
       </c>
       <c r="B26" s="8">
-        <v>292.35000000000002</v>
+        <v>227.7</v>
       </c>
       <c r="C26" s="10">
-        <v>267</v>
+        <v>207.1</v>
       </c>
       <c r="D26" s="13"/>
       <c r="E26" s="5"/>
@@ -4531,10 +5527,10 @@
         <v>31</v>
       </c>
       <c r="B27" s="8">
-        <v>335.75</v>
+        <v>262.60000000000002</v>
       </c>
       <c r="C27" s="10">
-        <v>306.8</v>
+        <v>250.25</v>
       </c>
       <c r="D27" s="13"/>
       <c r="E27" s="5"/>
@@ -4546,10 +5542,10 @@
         <v>32</v>
       </c>
       <c r="B28" s="8">
-        <v>5514.1</v>
+        <v>5008.7</v>
       </c>
       <c r="C28" s="10">
-        <v>5311.45</v>
+        <v>4912</v>
       </c>
       <c r="D28" s="13"/>
       <c r="E28" s="5"/>
@@ -4561,10 +5557,10 @@
         <v>33</v>
       </c>
       <c r="B29" s="8">
-        <v>652.45000000000005</v>
+        <v>760.5</v>
       </c>
       <c r="C29" s="10">
-        <v>638.1</v>
+        <v>735.05</v>
       </c>
       <c r="D29" s="13"/>
       <c r="E29" s="5"/>
@@ -4576,10 +5572,10 @@
         <v>34</v>
       </c>
       <c r="B30" s="8">
-        <v>120.6</v>
+        <v>554</v>
       </c>
       <c r="C30" s="10">
-        <v>116.5</v>
+        <v>529.75</v>
       </c>
       <c r="D30" s="13"/>
       <c r="E30" s="5"/>
@@ -4591,10 +5587,10 @@
         <v>35</v>
       </c>
       <c r="B31" s="8">
-        <v>770</v>
+        <v>734.35</v>
       </c>
       <c r="C31" s="10">
-        <v>747.6</v>
+        <v>709.15</v>
       </c>
       <c r="D31" s="13"/>
       <c r="E31" s="5"/>
@@ -4606,10 +5602,10 @@
         <v>36</v>
       </c>
       <c r="B32" s="8">
-        <v>406.45</v>
+        <v>350.9</v>
       </c>
       <c r="C32" s="10">
-        <v>390.3</v>
+        <v>339.5</v>
       </c>
       <c r="D32" s="13"/>
       <c r="E32" s="5"/>
@@ -4621,10 +5617,10 @@
         <v>37</v>
       </c>
       <c r="B33" s="8">
-        <v>1623</v>
+        <v>1086</v>
       </c>
       <c r="C33" s="10">
-        <v>1576.1</v>
+        <v>1055.6500000000001</v>
       </c>
       <c r="D33" s="13"/>
       <c r="E33" s="5"/>
@@ -4636,10 +5632,10 @@
         <v>38</v>
       </c>
       <c r="B34" s="8">
-        <v>1501</v>
+        <v>1496.2</v>
       </c>
       <c r="C34" s="10">
-        <v>1464</v>
+        <v>1466.05</v>
       </c>
       <c r="D34" s="13"/>
       <c r="E34" s="5"/>
@@ -4651,10 +5647,10 @@
         <v>39</v>
       </c>
       <c r="B35" s="8">
-        <v>5272.2</v>
+        <v>6137.35</v>
       </c>
       <c r="C35" s="10">
-        <v>5174.05</v>
+        <v>6008.3</v>
       </c>
       <c r="D35" s="13"/>
       <c r="E35" s="5"/>
@@ -4666,10 +5662,10 @@
         <v>40</v>
       </c>
       <c r="B36" s="8">
-        <v>1074.3</v>
+        <v>872.4</v>
       </c>
       <c r="C36" s="10">
-        <v>1005.1</v>
+        <v>845</v>
       </c>
       <c r="D36" s="13"/>
       <c r="E36" s="5"/>
@@ -4681,10 +5677,10 @@
         <v>41</v>
       </c>
       <c r="B37" s="8">
-        <v>1395</v>
+        <v>1110</v>
       </c>
       <c r="C37" s="10">
-        <v>1359.55</v>
+        <v>1059.75</v>
       </c>
       <c r="D37" s="13"/>
       <c r="E37" s="5"/>
@@ -4696,10 +5692,10 @@
         <v>42</v>
       </c>
       <c r="B38" s="8">
-        <v>435</v>
+        <v>285.8</v>
       </c>
       <c r="C38" s="10">
-        <v>415.2</v>
+        <v>274.35000000000002</v>
       </c>
       <c r="D38" s="13"/>
       <c r="E38" s="5"/>
@@ -4711,10 +5707,10 @@
         <v>43</v>
       </c>
       <c r="B39" s="8">
-        <v>3569</v>
+        <v>2737.1</v>
       </c>
       <c r="C39" s="10">
-        <v>3412.2</v>
+        <v>2678.5</v>
       </c>
       <c r="D39" s="13"/>
       <c r="E39" s="5"/>
@@ -4726,10 +5722,10 @@
         <v>44</v>
       </c>
       <c r="B40" s="8">
-        <v>605.29999999999995</v>
+        <v>530.35</v>
       </c>
       <c r="C40" s="10">
-        <v>582.04999999999995</v>
+        <v>524.25</v>
       </c>
       <c r="D40" s="13"/>
       <c r="E40" s="5"/>
@@ -4741,10 +5737,10 @@
         <v>45</v>
       </c>
       <c r="B41" s="8">
-        <v>1779.8</v>
+        <v>1893.9</v>
       </c>
       <c r="C41" s="10">
-        <v>1741.6</v>
+        <v>1854.7</v>
       </c>
       <c r="D41" s="13"/>
       <c r="E41" s="5"/>
@@ -4756,10 +5752,10 @@
         <v>46</v>
       </c>
       <c r="B42" s="8">
-        <v>1134.2</v>
+        <v>495.5</v>
       </c>
       <c r="C42" s="10">
-        <v>1070</v>
+        <v>466.1</v>
       </c>
       <c r="D42" s="13"/>
       <c r="E42" s="5"/>
@@ -4771,10 +5767,10 @@
         <v>47</v>
       </c>
       <c r="B43" s="8">
-        <v>2286.9499999999998</v>
+        <v>2123.5500000000002</v>
       </c>
       <c r="C43" s="10">
-        <v>2225</v>
+        <v>2080</v>
       </c>
       <c r="D43" s="13"/>
       <c r="E43" s="5"/>
@@ -4786,10 +5782,10 @@
         <v>48</v>
       </c>
       <c r="B44" s="8">
-        <v>116.2</v>
+        <v>127.7</v>
       </c>
       <c r="C44" s="10">
-        <v>113.5</v>
+        <v>122.75</v>
       </c>
       <c r="D44" s="13"/>
       <c r="E44" s="5"/>
@@ -4801,10 +5797,10 @@
         <v>49</v>
       </c>
       <c r="B45" s="8">
-        <v>4500</v>
+        <v>3524.7</v>
       </c>
       <c r="C45" s="10">
-        <v>4366.6000000000004</v>
+        <v>3455.05</v>
       </c>
       <c r="D45" s="13"/>
       <c r="E45" s="5"/>
@@ -4816,10 +5812,10 @@
         <v>50</v>
       </c>
       <c r="B46" s="8">
-        <v>9857.9500000000007</v>
+        <v>6979.95</v>
       </c>
       <c r="C46" s="10">
-        <v>9458.9</v>
+        <v>6722</v>
       </c>
       <c r="D46" s="13"/>
       <c r="E46" s="5"/>
@@ -4831,10 +5827,10 @@
         <v>51</v>
       </c>
       <c r="B47" s="8">
-        <v>835.95</v>
+        <v>848.75</v>
       </c>
       <c r="C47" s="10">
-        <v>799</v>
+        <v>809.3</v>
       </c>
       <c r="D47" s="13"/>
       <c r="E47" s="5"/>
@@ -4846,10 +5842,10 @@
         <v>52</v>
       </c>
       <c r="B48" s="8">
-        <v>5926</v>
+        <v>6308.55</v>
       </c>
       <c r="C48" s="10">
-        <v>5781.6</v>
+        <v>6214.5</v>
       </c>
       <c r="D48" s="13"/>
       <c r="E48" s="5"/>
@@ -4861,10 +5857,10 @@
         <v>53</v>
       </c>
       <c r="B49" s="8">
-        <v>4038.85</v>
+        <v>2773.95</v>
       </c>
       <c r="C49" s="10">
-        <v>3910.05</v>
+        <v>2682.5</v>
       </c>
       <c r="D49" s="13"/>
       <c r="E49" s="5"/>
@@ -4876,10 +5872,10 @@
         <v>54</v>
       </c>
       <c r="B50" s="8">
-        <v>536.70000000000005</v>
+        <v>306.8</v>
       </c>
       <c r="C50" s="10">
-        <v>492.1</v>
+        <v>298.85000000000002</v>
       </c>
       <c r="D50" s="13"/>
       <c r="E50" s="5"/>
@@ -4891,10 +5887,10 @@
         <v>55</v>
       </c>
       <c r="B51" s="8">
-        <v>1216.1500000000001</v>
+        <v>943.85</v>
       </c>
       <c r="C51" s="10">
-        <v>1164.25</v>
+        <v>912.05</v>
       </c>
       <c r="D51" s="13"/>
       <c r="E51" s="5"/>
@@ -4906,10 +5902,10 @@
         <v>56</v>
       </c>
       <c r="B52" s="8">
-        <v>871.8</v>
+        <v>752</v>
       </c>
       <c r="C52" s="10">
-        <v>840.05</v>
+        <v>715.6</v>
       </c>
       <c r="D52" s="13"/>
       <c r="E52" s="5"/>
@@ -4921,10 +5917,10 @@
         <v>57</v>
       </c>
       <c r="B53" s="8">
-        <v>700.95</v>
+        <v>630.9</v>
       </c>
       <c r="C53" s="10">
-        <v>675.2</v>
+        <v>606</v>
       </c>
       <c r="D53" s="13"/>
       <c r="E53" s="5"/>
@@ -4936,10 +5932,10 @@
         <v>58</v>
       </c>
       <c r="B54" s="8">
-        <v>1427.25</v>
+        <v>1223.8</v>
       </c>
       <c r="C54" s="10">
-        <v>1376</v>
+        <v>1203.7</v>
       </c>
       <c r="D54" s="13"/>
       <c r="E54" s="5"/>
@@ -4951,10 +5947,10 @@
         <v>59</v>
       </c>
       <c r="B55" s="8">
-        <v>2825.9</v>
+        <v>2234.1999999999998</v>
       </c>
       <c r="C55" s="10">
-        <v>2690</v>
+        <v>2157.9499999999998</v>
       </c>
       <c r="D55" s="13"/>
       <c r="E55" s="5"/>
@@ -4966,10 +5962,10 @@
         <v>60</v>
       </c>
       <c r="B56" s="8">
-        <v>471.4</v>
+        <v>424.85</v>
       </c>
       <c r="C56" s="10">
-        <v>440.1</v>
+        <v>410.4</v>
       </c>
       <c r="D56" s="13"/>
       <c r="E56" s="5"/>
@@ -4981,10 +5977,10 @@
         <v>61</v>
       </c>
       <c r="B57" s="8">
-        <v>2353</v>
+        <v>2208.9</v>
       </c>
       <c r="C57" s="10">
-        <v>2293.1</v>
+        <v>2165.0500000000002</v>
       </c>
       <c r="D57" s="13"/>
       <c r="E57" s="5"/>
@@ -4996,10 +5992,10 @@
         <v>62</v>
       </c>
       <c r="B58" s="8">
-        <v>576</v>
+        <v>546.95000000000005</v>
       </c>
       <c r="C58" s="10">
-        <v>551.4</v>
+        <v>528.54999999999995</v>
       </c>
       <c r="D58" s="13"/>
       <c r="E58" s="5"/>
@@ -5011,10 +6007,10 @@
         <v>63</v>
       </c>
       <c r="B59" s="8">
-        <v>4446</v>
+        <v>3182.55</v>
       </c>
       <c r="C59" s="10">
-        <v>4398.05</v>
+        <v>3006</v>
       </c>
       <c r="D59" s="13"/>
       <c r="E59" s="5"/>
@@ -5026,10 +6022,10 @@
         <v>64</v>
       </c>
       <c r="B60" s="8">
-        <v>1875</v>
+        <v>1520.3</v>
       </c>
       <c r="C60" s="10">
-        <v>1810</v>
+        <v>1476.05</v>
       </c>
       <c r="D60" s="13"/>
       <c r="E60" s="5"/>
@@ -5041,10 +6037,10 @@
         <v>65</v>
       </c>
       <c r="B61" s="8">
-        <v>1399.8</v>
+        <v>1677</v>
       </c>
       <c r="C61" s="10">
-        <v>1350.9</v>
+        <v>1642.85</v>
       </c>
       <c r="D61" s="13"/>
       <c r="E61" s="5"/>
@@ -5056,10 +6052,10 @@
         <v>66</v>
       </c>
       <c r="B62" s="8">
-        <v>3809</v>
+        <v>3831.45</v>
       </c>
       <c r="C62" s="10">
-        <v>3701.1</v>
+        <v>3680</v>
       </c>
       <c r="D62" s="13"/>
       <c r="E62" s="5"/>
@@ -5071,10 +6067,10 @@
         <v>67</v>
       </c>
       <c r="B63" s="8">
-        <v>558.75</v>
+        <v>634.79999999999995</v>
       </c>
       <c r="C63" s="10">
-        <v>550.4</v>
+        <v>611.29999999999995</v>
       </c>
       <c r="D63" s="13"/>
       <c r="E63" s="5"/>
@@ -5086,10 +6082,10 @@
         <v>68</v>
       </c>
       <c r="B64" s="8">
-        <v>695</v>
+        <v>534.04999999999995</v>
       </c>
       <c r="C64" s="10">
-        <v>673</v>
+        <v>517.5</v>
       </c>
       <c r="D64" s="13"/>
       <c r="E64" s="5"/>
@@ -5101,10 +6097,10 @@
         <v>69</v>
       </c>
       <c r="B65" s="8">
-        <v>350.7</v>
+        <v>275.60000000000002</v>
       </c>
       <c r="C65" s="10">
-        <v>324.35000000000002</v>
+        <v>255.75</v>
       </c>
       <c r="D65" s="13"/>
       <c r="E65" s="5"/>
@@ -5115,11 +6111,11 @@
       <c r="A66" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="B66" s="8">
-        <v>2214.25</v>
-      </c>
-      <c r="C66" s="10">
-        <v>2145</v>
+      <c r="B66" s="19">
+        <v>1688.75</v>
+      </c>
+      <c r="C66" s="20">
+        <v>1633.05</v>
       </c>
       <c r="D66" s="13"/>
       <c r="E66" s="5"/>
@@ -5131,10 +6127,10 @@
         <v>71</v>
       </c>
       <c r="B67" s="8">
-        <v>796.8</v>
+        <v>579</v>
       </c>
       <c r="C67" s="10">
-        <v>763.55</v>
+        <v>563</v>
       </c>
       <c r="D67" s="13"/>
       <c r="E67" s="5"/>
@@ -5146,10 +6142,10 @@
         <v>72</v>
       </c>
       <c r="B68" s="8">
-        <v>167.5</v>
+        <v>138.25</v>
       </c>
       <c r="C68" s="10">
-        <v>160.6</v>
+        <v>133.4</v>
       </c>
       <c r="D68" s="13"/>
       <c r="E68" s="5"/>
@@ -5161,10 +6157,10 @@
         <v>73</v>
       </c>
       <c r="B69" s="8">
-        <v>466.55</v>
+        <v>414</v>
       </c>
       <c r="C69" s="10">
-        <v>452</v>
+        <v>404</v>
       </c>
       <c r="D69" s="13"/>
       <c r="E69" s="5"/>
@@ -5176,10 +6172,10 @@
         <v>74</v>
       </c>
       <c r="B70" s="8">
-        <v>584.79999999999995</v>
+        <v>565.9</v>
       </c>
       <c r="C70" s="10">
-        <v>572.85</v>
+        <v>549.95000000000005</v>
       </c>
       <c r="D70" s="13"/>
       <c r="E70" s="5"/>
@@ -5191,10 +6187,10 @@
         <v>75</v>
       </c>
       <c r="B71" s="8">
-        <v>208.4</v>
+        <v>207</v>
       </c>
       <c r="C71" s="10">
-        <v>197.8</v>
+        <v>199.2</v>
       </c>
       <c r="D71" s="13"/>
       <c r="E71" s="5"/>
@@ -5206,10 +6202,10 @@
         <v>76</v>
       </c>
       <c r="B72" s="8">
-        <v>2559.5</v>
+        <v>2661.8</v>
       </c>
       <c r="C72" s="10">
-        <v>2508.0500000000002</v>
+        <v>2599.25</v>
       </c>
       <c r="D72" s="13"/>
       <c r="E72" s="5"/>
@@ -5221,10 +6217,10 @@
         <v>77</v>
       </c>
       <c r="B73" s="8">
-        <v>4357</v>
+        <v>3215.9</v>
       </c>
       <c r="C73" s="10">
-        <v>4260</v>
+        <v>3135</v>
       </c>
       <c r="D73" s="13"/>
       <c r="E73" s="5"/>
@@ -5236,10 +6232,10 @@
         <v>78</v>
       </c>
       <c r="B74" s="8">
-        <v>1509.8</v>
+        <v>1489.5</v>
       </c>
       <c r="C74" s="10">
-        <v>1470.9</v>
+        <v>1456.7</v>
       </c>
       <c r="D74" s="13"/>
       <c r="E74" s="5"/>
@@ -5251,10 +6247,10 @@
         <v>79</v>
       </c>
       <c r="B75" s="8">
-        <v>344.95</v>
+        <v>252.4</v>
       </c>
       <c r="C75" s="10">
-        <v>334.5</v>
+        <v>241.2</v>
       </c>
       <c r="D75" s="13"/>
       <c r="E75" s="5"/>
@@ -5266,10 +6262,10 @@
         <v>80</v>
       </c>
       <c r="B76" s="8">
-        <v>961.8</v>
+        <v>1199</v>
       </c>
       <c r="C76" s="10">
-        <v>906.6</v>
+        <v>1101</v>
       </c>
       <c r="D76" s="13"/>
       <c r="E76" s="5"/>
@@ -5281,10 +6277,10 @@
         <v>81</v>
       </c>
       <c r="B77" s="8">
-        <v>1179.95</v>
+        <v>1194.9000000000001</v>
       </c>
       <c r="C77" s="10">
-        <v>1150</v>
+        <v>1143.9000000000001</v>
       </c>
       <c r="D77" s="13"/>
       <c r="E77" s="5"/>
@@ -5296,10 +6292,10 @@
         <v>82</v>
       </c>
       <c r="B78" s="8">
-        <v>1035</v>
+        <v>783.1</v>
       </c>
       <c r="C78" s="10">
-        <v>1000</v>
+        <v>760.9</v>
       </c>
       <c r="D78" s="13"/>
       <c r="E78" s="5"/>
@@ -5311,10 +6307,10 @@
         <v>83</v>
       </c>
       <c r="B79" s="8">
-        <v>4027.75</v>
+        <v>4122.1499999999996</v>
       </c>
       <c r="C79" s="10">
-        <v>3900.95</v>
+        <v>4010.05</v>
       </c>
       <c r="D79" s="13"/>
       <c r="E79" s="5"/>
@@ -5326,10 +6322,10 @@
         <v>84</v>
       </c>
       <c r="B80" s="8">
-        <v>892.9</v>
+        <v>790.2</v>
       </c>
       <c r="C80" s="10">
-        <v>877.5</v>
+        <v>774.55</v>
       </c>
       <c r="D80" s="13"/>
       <c r="E80" s="5"/>
@@ -5341,10 +6337,10 @@
         <v>85</v>
       </c>
       <c r="B81" s="8">
-        <v>537.25</v>
+        <v>453.25</v>
       </c>
       <c r="C81" s="10">
-        <v>515.5</v>
+        <v>439.9</v>
       </c>
       <c r="D81" s="13"/>
       <c r="E81" s="5"/>
@@ -5356,10 +6352,10 @@
         <v>86</v>
       </c>
       <c r="B82" s="8">
-        <v>1738.5</v>
+        <v>1756</v>
       </c>
       <c r="C82" s="10">
-        <v>1703.8</v>
+        <v>1721.2</v>
       </c>
       <c r="D82" s="13"/>
       <c r="E82" s="5"/>
@@ -5371,10 +6367,10 @@
         <v>87</v>
       </c>
       <c r="B83" s="8">
-        <v>2822</v>
+        <v>2065</v>
       </c>
       <c r="C83" s="10">
-        <v>2705.55</v>
+        <v>2013.2</v>
       </c>
       <c r="D83" s="13"/>
       <c r="E83" s="5"/>
@@ -5386,10 +6382,10 @@
         <v>88</v>
       </c>
       <c r="B84" s="8">
-        <v>440</v>
+        <v>403.1</v>
       </c>
       <c r="C84" s="10">
-        <v>425.55</v>
+        <v>389.5</v>
       </c>
       <c r="D84" s="13"/>
       <c r="E84" s="5"/>
@@ -5401,10 +6397,10 @@
         <v>89</v>
       </c>
       <c r="B85" s="8">
-        <v>654</v>
+        <v>594.75</v>
       </c>
       <c r="C85" s="10">
-        <v>629.4</v>
+        <v>575.25</v>
       </c>
       <c r="D85" s="13"/>
       <c r="E85" s="5"/>
@@ -5416,10 +6412,10 @@
         <v>90</v>
       </c>
       <c r="B86" s="8">
-        <v>4819</v>
+        <v>5249.95</v>
       </c>
       <c r="C86" s="10">
-        <v>4703</v>
+        <v>5170</v>
       </c>
       <c r="D86" s="13"/>
       <c r="E86" s="5"/>
@@ -5431,10 +6427,10 @@
         <v>91</v>
       </c>
       <c r="B87" s="8">
-        <v>4707</v>
+        <v>5437.85</v>
       </c>
       <c r="C87" s="10">
-        <v>4641</v>
+        <v>5242.2</v>
       </c>
       <c r="D87" s="13"/>
       <c r="E87" s="5"/>
@@ -5446,10 +6442,10 @@
         <v>92</v>
       </c>
       <c r="B88" s="8">
-        <v>1645.45</v>
+        <v>1674</v>
       </c>
       <c r="C88" s="10">
-        <v>1601.25</v>
+        <v>1614</v>
       </c>
       <c r="D88" s="13"/>
       <c r="E88" s="5"/>
@@ -5461,10 +6457,10 @@
         <v>93</v>
       </c>
       <c r="B89" s="8">
-        <v>339.9</v>
+        <v>269.7</v>
       </c>
       <c r="C89" s="10">
-        <v>328.05</v>
+        <v>260.10000000000002</v>
       </c>
       <c r="D89" s="13"/>
       <c r="E89" s="5"/>
@@ -5476,10 +6472,10 @@
         <v>94</v>
       </c>
       <c r="B90" s="8">
-        <v>178.8</v>
+        <v>167.35</v>
       </c>
       <c r="C90" s="10">
-        <v>170</v>
+        <v>161.65</v>
       </c>
       <c r="D90" s="13"/>
       <c r="E90" s="5"/>
@@ -5491,10 +6487,10 @@
         <v>95</v>
       </c>
       <c r="B91" s="8">
-        <v>650</v>
+        <v>509.65</v>
       </c>
       <c r="C91" s="10">
-        <v>626.54999999999995</v>
+        <v>496.5</v>
       </c>
       <c r="D91" s="13"/>
       <c r="E91" s="5"/>
@@ -5506,10 +6502,10 @@
         <v>96</v>
       </c>
       <c r="B92" s="8">
-        <v>1313.9</v>
+        <v>1162</v>
       </c>
       <c r="C92" s="10">
-        <v>1268.55</v>
+        <v>1108.45</v>
       </c>
       <c r="D92" s="13"/>
       <c r="E92" s="5"/>
@@ -5521,10 +6517,10 @@
         <v>97</v>
       </c>
       <c r="B93" s="8">
-        <v>3581</v>
+        <v>3277.45</v>
       </c>
       <c r="C93" s="10">
-        <v>3472.5</v>
+        <v>3075.25</v>
       </c>
       <c r="D93" s="13"/>
       <c r="E93" s="5"/>
@@ -5536,10 +6532,10 @@
         <v>98</v>
       </c>
       <c r="B94" s="8">
-        <v>2067.9499999999998</v>
+        <v>1627.95</v>
       </c>
       <c r="C94" s="10">
-        <v>1996.1</v>
+        <v>1580.1</v>
       </c>
       <c r="D94" s="13"/>
       <c r="E94" s="5"/>
@@ -5551,10 +6547,10 @@
         <v>99</v>
       </c>
       <c r="B95" s="8">
-        <v>939</v>
+        <v>994</v>
       </c>
       <c r="C95" s="10">
-        <v>924.05</v>
+        <v>952.9</v>
       </c>
       <c r="D95" s="13"/>
       <c r="E95" s="5"/>
@@ -5566,10 +6562,10 @@
         <v>100</v>
       </c>
       <c r="B96" s="8">
-        <v>1950</v>
+        <v>1279.6500000000001</v>
       </c>
       <c r="C96" s="10">
-        <v>1912</v>
+        <v>1243</v>
       </c>
       <c r="D96" s="13"/>
       <c r="E96" s="5"/>
@@ -5581,10 +6577,10 @@
         <v>101</v>
       </c>
       <c r="B97" s="8">
-        <v>2474.4499999999998</v>
+        <v>2502</v>
       </c>
       <c r="C97" s="10">
-        <v>2399.8000000000002</v>
+        <v>2455.85</v>
       </c>
       <c r="D97" s="13"/>
       <c r="E97" s="5"/>
@@ -5596,10 +6592,10 @@
         <v>102</v>
       </c>
       <c r="B98" s="8">
-        <v>1810.95</v>
+        <v>1368.9</v>
       </c>
       <c r="C98" s="10">
-        <v>1740</v>
+        <v>1328.85</v>
       </c>
       <c r="D98" s="13"/>
       <c r="E98" s="5"/>
@@ -5611,10 +6607,10 @@
         <v>103</v>
       </c>
       <c r="B99" s="8">
-        <v>622</v>
+        <v>488.7</v>
       </c>
       <c r="C99" s="10">
-        <v>554.1</v>
+        <v>450.5</v>
       </c>
       <c r="D99" s="13"/>
       <c r="E99" s="5"/>
@@ -5626,10 +6622,10 @@
         <v>104</v>
       </c>
       <c r="B100" s="8">
-        <v>6164.45</v>
+        <v>5280</v>
       </c>
       <c r="C100" s="10">
-        <v>6000.8</v>
+        <v>5161.3</v>
       </c>
       <c r="D100" s="13"/>
       <c r="E100" s="5"/>
@@ -5641,10 +6637,10 @@
         <v>105</v>
       </c>
       <c r="B101" s="8">
-        <v>3351.85</v>
+        <v>3010.05</v>
       </c>
       <c r="C101" s="10">
-        <v>3285.2</v>
+        <v>2964.3</v>
       </c>
       <c r="D101" s="13"/>
       <c r="E101" s="5"/>
@@ -5656,10 +6652,10 @@
         <v>106</v>
       </c>
       <c r="B102" s="8">
-        <v>257.5</v>
+        <v>204.5</v>
       </c>
       <c r="C102" s="10">
-        <v>247</v>
+        <v>190.35</v>
       </c>
       <c r="D102" s="13"/>
       <c r="E102" s="5"/>
@@ -5671,10 +6667,10 @@
         <v>107</v>
       </c>
       <c r="B103" s="8">
-        <v>359.75</v>
+        <v>326.05</v>
       </c>
       <c r="C103" s="10">
-        <v>345</v>
+        <v>305.75</v>
       </c>
       <c r="D103" s="13"/>
       <c r="E103" s="5"/>
@@ -5686,10 +6682,10 @@
         <v>108</v>
       </c>
       <c r="B104" s="8">
-        <v>1913.25</v>
+        <v>1343.95</v>
       </c>
       <c r="C104" s="10">
-        <v>1845.15</v>
+        <v>1297.25</v>
       </c>
       <c r="D104" s="13"/>
       <c r="E104" s="5"/>
@@ -5701,10 +6697,10 @@
         <v>109</v>
       </c>
       <c r="B105" s="8">
-        <v>259.5</v>
+        <v>266.39999999999998</v>
       </c>
       <c r="C105" s="10">
-        <v>249.25</v>
+        <v>248.9</v>
       </c>
       <c r="D105" s="13"/>
       <c r="E105" s="5"/>
@@ -5716,10 +6712,10 @@
         <v>110</v>
       </c>
       <c r="B106" s="8">
-        <v>811</v>
+        <v>843.5</v>
       </c>
       <c r="C106" s="10">
-        <v>787.8</v>
+        <v>814.8</v>
       </c>
       <c r="D106" s="13"/>
       <c r="E106" s="5"/>
@@ -5731,10 +6727,10 @@
         <v>111</v>
       </c>
       <c r="B107" s="8">
-        <v>3714.8</v>
+        <v>8454.85</v>
       </c>
       <c r="C107" s="10">
-        <v>3612</v>
+        <v>8180</v>
       </c>
       <c r="D107" s="13"/>
       <c r="E107" s="5"/>
@@ -5746,10 +6742,10 @@
         <v>112</v>
       </c>
       <c r="B108" s="8">
-        <v>307</v>
+        <v>269.60000000000002</v>
       </c>
       <c r="C108" s="10">
-        <v>291.5</v>
+        <v>258.05</v>
       </c>
       <c r="D108" s="13"/>
       <c r="E108" s="5"/>
@@ -5761,10 +6757,10 @@
         <v>113</v>
       </c>
       <c r="B109" s="8">
-        <v>3164.55</v>
+        <v>2894</v>
       </c>
       <c r="C109" s="10">
-        <v>3084</v>
+        <v>2819</v>
       </c>
       <c r="D109" s="13"/>
       <c r="E109" s="5"/>
@@ -5776,10 +6772,10 @@
         <v>114</v>
       </c>
       <c r="B110" s="8">
-        <v>6980</v>
+        <v>4918.05</v>
       </c>
       <c r="C110" s="10">
-        <v>6808.2</v>
+        <v>4775</v>
       </c>
       <c r="D110" s="13"/>
       <c r="E110" s="5"/>
@@ -5791,10 +6787,10 @@
         <v>115</v>
       </c>
       <c r="B111" s="8">
-        <v>311.45</v>
+        <v>272</v>
       </c>
       <c r="C111" s="10">
-        <v>298.10000000000002</v>
+        <v>257.64999999999998</v>
       </c>
       <c r="D111" s="13"/>
       <c r="E111" s="5"/>
@@ -5806,10 +6802,10 @@
         <v>116</v>
       </c>
       <c r="B112" s="8">
-        <v>161.65</v>
+        <v>162.30000000000001</v>
       </c>
       <c r="C112" s="10">
-        <v>156.25</v>
+        <v>156.35</v>
       </c>
       <c r="D112" s="13"/>
       <c r="E112" s="5"/>
@@ -5821,10 +6817,10 @@
         <v>117</v>
       </c>
       <c r="B113" s="8">
-        <v>800.5</v>
+        <v>809</v>
       </c>
       <c r="C113" s="10">
-        <v>760</v>
+        <v>792.7</v>
       </c>
       <c r="D113" s="13"/>
       <c r="E113" s="5"/>
@@ -5836,10 +6832,10 @@
         <v>118</v>
       </c>
       <c r="B114" s="8">
-        <v>250.3</v>
+        <v>230.65</v>
       </c>
       <c r="C114" s="10">
-        <v>242.5</v>
+        <v>222.25</v>
       </c>
       <c r="D114" s="13"/>
       <c r="E114" s="5"/>
@@ -5851,10 +6847,10 @@
         <v>119</v>
       </c>
       <c r="B115" s="8">
-        <v>514.29999999999995</v>
+        <v>466.5</v>
       </c>
       <c r="C115" s="10">
-        <v>466.2</v>
+        <v>430.35</v>
       </c>
       <c r="D115" s="13"/>
       <c r="E115" s="5"/>
@@ -5866,10 +6862,10 @@
         <v>120</v>
       </c>
       <c r="B116" s="8">
-        <v>707</v>
+        <v>704.65</v>
       </c>
       <c r="C116" s="10">
-        <v>699.45</v>
+        <v>696</v>
       </c>
       <c r="D116" s="13"/>
       <c r="E116" s="5"/>
@@ -5881,10 +6877,10 @@
         <v>121</v>
       </c>
       <c r="B117" s="8">
-        <v>1445.8</v>
+        <v>1504.95</v>
       </c>
       <c r="C117" s="10">
-        <v>1380.25</v>
+        <v>1481.1</v>
       </c>
       <c r="D117" s="13"/>
       <c r="E117" s="5"/>
@@ -5896,10 +6892,10 @@
         <v>122</v>
       </c>
       <c r="B118" s="8">
-        <v>6838.4</v>
+        <v>4820.6000000000004</v>
       </c>
       <c r="C118" s="10">
-        <v>6595.05</v>
+        <v>4682.1000000000004</v>
       </c>
       <c r="D118" s="13"/>
       <c r="E118" s="5"/>
@@ -5911,10 +6907,10 @@
         <v>123</v>
       </c>
       <c r="B119" s="8">
-        <v>2312</v>
+        <v>2449.9</v>
       </c>
       <c r="C119" s="10">
-        <v>2279</v>
+        <v>2404.4</v>
       </c>
       <c r="D119" s="13"/>
       <c r="E119" s="5"/>
@@ -5926,10 +6922,10 @@
         <v>124</v>
       </c>
       <c r="B120" s="8">
-        <v>905</v>
+        <v>799.2</v>
       </c>
       <c r="C120" s="10">
-        <v>873.8</v>
+        <v>766.85</v>
       </c>
       <c r="D120" s="13"/>
       <c r="E120" s="5"/>
@@ -5941,10 +6937,10 @@
         <v>125</v>
       </c>
       <c r="B121" s="8">
-        <v>1494</v>
+        <v>1573.5</v>
       </c>
       <c r="C121" s="10">
-        <v>1455.05</v>
+        <v>1541.2</v>
       </c>
       <c r="D121" s="13"/>
       <c r="E121" s="5"/>
@@ -5956,10 +6952,10 @@
         <v>126</v>
       </c>
       <c r="B122" s="8">
-        <v>688</v>
+        <v>687.9</v>
       </c>
       <c r="C122" s="10">
-        <v>670.05</v>
+        <v>671.9</v>
       </c>
       <c r="D122" s="13"/>
       <c r="E122" s="5"/>
@@ -5971,10 +6967,10 @@
         <v>127</v>
       </c>
       <c r="B123" s="8">
-        <v>1799</v>
+        <v>1954.6</v>
       </c>
       <c r="C123" s="10">
-        <v>1748</v>
+        <v>1896.55</v>
       </c>
       <c r="D123" s="13"/>
       <c r="E123" s="5"/>
@@ -5986,10 +6982,10 @@
         <v>128</v>
       </c>
       <c r="B124" s="8">
-        <v>946</v>
+        <v>979.75</v>
       </c>
       <c r="C124" s="10">
-        <v>931.2</v>
+        <v>940</v>
       </c>
       <c r="D124" s="13"/>
       <c r="E124" s="5"/>
@@ -6001,10 +6997,10 @@
         <v>129</v>
       </c>
       <c r="B125" s="8">
-        <v>1323.6</v>
+        <v>1293</v>
       </c>
       <c r="C125" s="10">
-        <v>1274.2</v>
+        <v>1268.5</v>
       </c>
       <c r="D125" s="13"/>
       <c r="E125" s="5"/>
@@ -6016,10 +7012,10 @@
         <v>130</v>
       </c>
       <c r="B126" s="8">
-        <v>2830.95</v>
+        <v>2711.1</v>
       </c>
       <c r="C126" s="10">
-        <v>2745.35</v>
+        <v>2577</v>
       </c>
       <c r="D126" s="13"/>
       <c r="E126" s="5"/>
@@ -6031,10 +7027,10 @@
         <v>131</v>
       </c>
       <c r="B127" s="8">
-        <v>1478.15</v>
+        <v>1185</v>
       </c>
       <c r="C127" s="10">
-        <v>1441.1</v>
+        <v>1115.45</v>
       </c>
       <c r="D127" s="13"/>
       <c r="E127" s="5"/>
@@ -6046,10 +7042,10 @@
         <v>132</v>
       </c>
       <c r="B128" s="8">
-        <v>4928.6000000000004</v>
+        <v>4145</v>
       </c>
       <c r="C128" s="10">
-        <v>4821.05</v>
+        <v>3981.25</v>
       </c>
       <c r="D128" s="13"/>
       <c r="E128" s="5"/>
@@ -6061,10 +7057,10 @@
         <v>133</v>
       </c>
       <c r="B129" s="8">
-        <v>2409.9499999999998</v>
+        <v>2159</v>
       </c>
       <c r="C129" s="10">
-        <v>2335.5</v>
+        <v>2054.9499999999998</v>
       </c>
       <c r="D129" s="13"/>
       <c r="E129" s="5"/>
@@ -6076,10 +7072,10 @@
         <v>134</v>
       </c>
       <c r="B130" s="8">
-        <v>2046</v>
+        <v>1745.95</v>
       </c>
       <c r="C130" s="10">
-        <v>1965.65</v>
+        <v>1696.25</v>
       </c>
       <c r="D130" s="13"/>
       <c r="E130" s="5"/>
@@ -6091,10 +7087,10 @@
         <v>135</v>
       </c>
       <c r="B131" s="8">
-        <v>10176.5</v>
+        <v>9750.9</v>
       </c>
       <c r="C131" s="10">
-        <v>9931.1</v>
+        <v>9543.7999999999993</v>
       </c>
       <c r="D131" s="13"/>
       <c r="E131" s="5"/>
@@ -6106,10 +7102,10 @@
         <v>136</v>
       </c>
       <c r="B132" s="8">
-        <v>545.5</v>
+        <v>477.5</v>
       </c>
       <c r="C132" s="10">
-        <v>527.70000000000005</v>
+        <v>459.45</v>
       </c>
       <c r="D132" s="13"/>
       <c r="E132" s="5"/>
@@ -6121,10 +7117,10 @@
         <v>137</v>
       </c>
       <c r="B133" s="8">
-        <v>458</v>
+        <v>266</v>
       </c>
       <c r="C133" s="10">
-        <v>446.3</v>
+        <v>255.15</v>
       </c>
       <c r="D133" s="13"/>
       <c r="E133" s="5"/>
@@ -6136,10 +7132,10 @@
         <v>138</v>
       </c>
       <c r="B134" s="8">
-        <v>1478.2</v>
+        <v>1073.6500000000001</v>
       </c>
       <c r="C134" s="10">
-        <v>1440</v>
+        <v>1050.05</v>
       </c>
       <c r="D134" s="13"/>
       <c r="E134" s="5"/>
@@ -6151,10 +7147,10 @@
         <v>139</v>
       </c>
       <c r="B135" s="8">
-        <v>157.55000000000001</v>
+        <v>149.1</v>
       </c>
       <c r="C135" s="10">
-        <v>150.25</v>
+        <v>141</v>
       </c>
       <c r="D135" s="13"/>
       <c r="E135" s="5"/>
@@ -6165,16 +7161,44 @@
       <c r="A136" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="B136" s="18">
-        <v>1062.95</v>
-      </c>
-      <c r="C136" s="11">
-        <v>1033.95</v>
+      <c r="B136" s="8">
+        <v>994.65</v>
+      </c>
+      <c r="C136" s="10">
+        <v>971.25</v>
       </c>
       <c r="D136" s="14"/>
       <c r="E136" s="6"/>
       <c r="F136" s="17"/>
       <c r="G136" s="6"/>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B137" s="8"/>
+      <c r="C137" s="10"/>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B138" s="8"/>
+      <c r="C138" s="10"/>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B139" s="8"/>
+      <c r="C139" s="10"/>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B140" s="8"/>
+      <c r="C140" s="10"/>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B141" s="8"/>
+      <c r="C141" s="10"/>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B142" s="8"/>
+      <c r="C142" s="10"/>
+    </row>
+    <row r="143" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B143" s="18"/>
+      <c r="C143" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>